<commit_message>
Draft UI and con't Algo
</commit_message>
<xml_diff>
--- a/app/algorithm/data.xlsx
+++ b/app/algorithm/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\Chatbot\app\algorithm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\IAI\app\algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFA62FE-D554-463A-B4AD-A3662BBFE572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641E8848-71AB-4A04-9968-6AD9CBC72249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="852" windowWidth="11796" windowHeight="11880" xr2:uid="{F56ACAE5-2C64-4881-A454-41EAB5000D3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F56ACAE5-2C64-4881-A454-41EAB5000D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>